<commit_message>
1/12 beta test update
</commit_message>
<xml_diff>
--- a/beta_test/test.xlsx
+++ b/beta_test/test.xlsx
@@ -1146,7 +1146,7 @@
         <v/>
       </c>
       <c r="E15" s="30" t="n">
-        <v>130.73</v>
+        <v>133.49</v>
       </c>
       <c r="F15" s="10">
         <f>(E15-C3)/C3</f>
@@ -1169,11 +1169,7 @@
           <t>일간 등락률</t>
         </is>
       </c>
-      <c r="M15" s="17" t="inlineStr">
-        <is>
-          <t xml:space="preserve">AAPL has a big change. 10%    GOOGL has a big change. 10%    NVDA has a big change. 10%    </t>
-        </is>
-      </c>
+      <c r="M15" s="17" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="B16" s="14" t="inlineStr">
@@ -1189,7 +1185,7 @@
         <v/>
       </c>
       <c r="E16" s="30" t="n">
-        <v>88.42</v>
+        <v>91.52</v>
       </c>
       <c r="F16" s="10">
         <f>(E16-C4)/C4</f>
@@ -1214,7 +1210,7 @@
       </c>
       <c r="M16" s="17" t="inlineStr">
         <is>
-          <t xml:space="preserve">AAPL is arrived new node. -27%    GOOGL is arrived new node. -42%    NVDA is arrived new node. -45%    </t>
+          <t xml:space="preserve">TSLA is arrived new node. -68%    </t>
         </is>
       </c>
     </row>
@@ -1232,7 +1228,7 @@
         <v/>
       </c>
       <c r="E17" s="31" t="n">
-        <v>159.09</v>
+        <v>160.01</v>
       </c>
       <c r="F17" s="10">
         <f>(E17-C5)/C5</f>
@@ -1255,7 +1251,7 @@
           <t>금리 관련</t>
         </is>
       </c>
-      <c r="M17" s="17" t="n"/>
+      <c r="M17" s="17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="B18" s="11" t="inlineStr">
@@ -1271,7 +1267,7 @@
         <v/>
       </c>
       <c r="E18" s="30" t="n">
-        <v>118.85</v>
+        <v>123.22</v>
       </c>
       <c r="F18" s="10">
         <f>(E18-C6)/C6</f>
@@ -1310,7 +1306,7 @@
         <v/>
       </c>
       <c r="E19" s="30" t="n">
-        <v>62.13</v>
+        <v>62.01</v>
       </c>
       <c r="F19" s="10">
         <f>(E19-C7)/C7</f>
@@ -1343,7 +1339,7 @@
         <v/>
       </c>
       <c r="E20" s="30" t="n">
-        <v>177.85</v>
+        <v>178.05</v>
       </c>
       <c r="F20" s="10">
         <f>(E20-C8)/C8</f>
@@ -1376,7 +1372,7 @@
         <v/>
       </c>
       <c r="E21" s="30" t="n">
-        <v>582.7</v>
+        <v>592.7</v>
       </c>
       <c r="F21" s="10">
         <f>(E21-C9)/C9</f>
@@ -1404,7 +1400,7 @@
         <v/>
       </c>
       <c r="E22" s="30" t="n">
-        <v>272.83</v>
+        <v>277.55</v>
       </c>
       <c r="F22" s="10">
         <f>(E22-$A$22)/$A$22</f>
@@ -1432,7 +1428,7 @@
         <v/>
       </c>
       <c r="E23" s="30" t="n">
-        <v>390.58</v>
+        <v>395.52</v>
       </c>
       <c r="F23" s="10">
         <f>(E23-$A$24)/$A$24</f>

</xml_diff>